<commit_message>
update to order schedule page
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderSchedulePage, Steven Kennedy.xlsx
+++ b/Testing Spreadsheet v1.0 OrderSchedulePage, Steven Kennedy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="16560" windowHeight="6285" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="16560" windowHeight="6285" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="334">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -1200,6 +1200,39 @@
   </si>
   <si>
     <t>All contents of the Schedule Order page are easy to read and function correctly using this browser</t>
+  </si>
+  <si>
+    <t>ScheduleOrder_39</t>
+  </si>
+  <si>
+    <t>ScheduleOrder_40</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 25 December '15, Hour: 11, Minute: 00</t>
+  </si>
+  <si>
+    <t>Schedule_Time_12</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 06 April '15, Hour: 15, Minute: 45</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_39</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_40</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set order date to Christmas Day.</t>
+  </si>
+  <si>
+    <t>Denied order. Order is void due to this being a public holiday.</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set order date to Easter Monday.</t>
+  </si>
+  <si>
+    <t>Order complete. Order Receipt Page appears  due to being open on this public holiday.</t>
   </si>
 </sst>
 </file>
@@ -1549,7 +1582,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1559,7 +1591,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1569,7 +1600,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1608,10 +1638,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1634,7 +1664,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1731,11 +1760,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="87948288"/>
-        <c:axId val="87962368"/>
+        <c:axId val="88449024"/>
+        <c:axId val="88450560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87948288"/>
+        <c:axId val="88449024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +1773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87962368"/>
+        <c:crossAx val="88450560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1752,7 +1781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87962368"/>
+        <c:axId val="88450560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87948288"/>
+        <c:crossAx val="88449024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2171,8 +2200,8 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,8 +2549,8 @@
   </sheetPr>
   <dimension ref="A1:Z176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView topLeftCell="A34" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3470,7 +3499,7 @@
       </c>
       <c r="U22" s="31">
         <f>COUNTIF(H2:H105,"*Passed*")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -3532,7 +3561,7 @@
       </c>
       <c r="U24" s="31">
         <f>COUNTIF(H4:H105,"*Failed*")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="57" x14ac:dyDescent="0.25">
@@ -4131,18 +4160,50 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E41" s="10"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
+    <row r="41" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="13">
+        <v>42097</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M41" s="33">
+        <v>42097</v>
+      </c>
       <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
+      <c r="O41" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="P41" s="10"/>
       <c r="T41" t="s">
         <v>34</v>
@@ -4152,18 +4213,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E42" s="10"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
+    <row r="42" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" s="13">
+        <v>42097</v>
+      </c>
+      <c r="H42" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J42" s="3"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="33"/>
       <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
+      <c r="O42" s="3"/>
       <c r="P42" s="10"/>
       <c r="T42" t="s">
         <v>57</v>
@@ -6099,13 +6182,13 @@
           <x14:formula1>
             <xm:f>Settings!$F$4:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L21 L26</xm:sqref>
+          <xm:sqref>L2:L21 L26 L41:L42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K26</xm:sqref>
+          <xm:sqref>K2:K26 K41:K42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6118,10 +6201,10 @@
   <sheetPr>
     <tabColor rgb="FF99FF99"/>
   </sheetPr>
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6950,6 +7033,40 @@
       </c>
       <c r="E39" s="1" t="s">
         <v>322</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -7044,6 +7161,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -7157,22 +7289,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7186,27 +7326,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change to schedule order page
-changes made
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderSchedulePage, Steven Kennedy.xlsx
+++ b/Testing Spreadsheet v1.0 OrderSchedulePage, Steven Kennedy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="16560" windowHeight="6285" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="16560" windowHeight="6285" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="343">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -1019,9 +1019,6 @@
     <t>Requirements 3.2.2</t>
   </si>
   <si>
-    <t>To check the company lgog is displayed at the header of the Schedule page</t>
-  </si>
-  <si>
     <t>To check that the footer of the Schedule web page has copyright and site version information</t>
   </si>
   <si>
@@ -1233,6 +1230,36 @@
   </si>
   <si>
     <t>Order complete. Order Receipt Page appears  due to being open on this public holiday.</t>
+  </si>
+  <si>
+    <t>To check the company logo is displayed at the header of the Schedule page</t>
+  </si>
+  <si>
+    <t>Display Schedule page on a Google Nexus 10</t>
+  </si>
+  <si>
+    <t>Display Schedule page on a Samsung Galaxy  S4</t>
+  </si>
+  <si>
+    <t>ScheduleOrder_41</t>
+  </si>
+  <si>
+    <t>ScheduleOrder_42</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_41</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_42</t>
+  </si>
+  <si>
+    <t>Test Schedule Order page on a Google Nexus 10 device</t>
+  </si>
+  <si>
+    <t>Test Schedule Order page on a Samsung Galaxy S4 device</t>
+  </si>
+  <si>
+    <t>Logo does appear; although a water mark has been left within the logo image</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1665,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12</c:v>
@@ -1705,7 +1732,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Test Cases'!$T$41:$T$45</c:f>
+              <c:f>'Test Cases'!$T$43:$T$47</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1728,7 +1755,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Test Cases'!$U$41:$U$45</c:f>
+              <c:f>'Test Cases'!$U$43:$U$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1760,11 +1787,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="88449024"/>
-        <c:axId val="88450560"/>
+        <c:axId val="84214144"/>
+        <c:axId val="84215680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88449024"/>
+        <c:axId val="84214144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1773,7 +1800,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88450560"/>
+        <c:crossAx val="84215680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1781,7 +1808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88450560"/>
+        <c:axId val="84215680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1792,7 +1819,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88449024"/>
+        <c:crossAx val="84214144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1845,13 +1872,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>21166</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>325966</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2200,8 +2227,8 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2361,7 +2388,7 @@
         <v>222</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>262</v>
+        <v>333</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>251</v>
@@ -2375,7 +2402,7 @@
         <v>223</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>252</v>
@@ -2389,7 +2416,7 @@
         <v>224</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>253</v>
@@ -2403,7 +2430,7 @@
         <v>225</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>254</v>
@@ -2417,7 +2444,7 @@
         <v>226</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>255</v>
@@ -2431,7 +2458,7 @@
         <v>227</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>256</v>
@@ -2445,7 +2472,7 @@
         <v>228</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>257</v>
@@ -2459,7 +2486,7 @@
         <v>229</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>258</v>
@@ -2473,7 +2500,7 @@
         <v>230</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>259</v>
@@ -2487,7 +2514,7 @@
         <v>231</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>260</v>
@@ -2501,7 +2528,7 @@
         <v>232</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>261</v>
@@ -2515,7 +2542,7 @@
         <v>233</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>261</v>
@@ -2547,10 +2574,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:Z176"/>
+  <dimension ref="A1:Z178"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView topLeftCell="A21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3498,8 +3525,8 @@
         <v>53</v>
       </c>
       <c r="U22" s="31">
-        <f>COUNTIF(H2:H105,"*Passed*")</f>
-        <v>27</v>
+        <f>COUNTIF(H2:H107,"*Passed*")</f>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -3560,7 +3587,7 @@
         <v>25</v>
       </c>
       <c r="U24" s="31">
-        <f>COUNTIF(H4:H105,"*Failed*")</f>
+        <f>COUNTIF(H4:H107,"*Failed*")</f>
         <v>12</v>
       </c>
     </row>
@@ -3603,7 +3630,7 @@
         <v>54</v>
       </c>
       <c r="U25" s="31">
-        <f>COUNTIF(H11:H105,"*Not*")</f>
+        <f>COUNTIF(H11:H107,"*Not*")</f>
         <v>0</v>
       </c>
     </row>
@@ -3636,7 +3663,7 @@
         <v>66</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>33</v>
@@ -3649,7 +3676,7 @@
       </c>
       <c r="N26" s="10"/>
       <c r="O26" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P26" s="10"/>
     </row>
@@ -4049,27 +4076,27 @@
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
     </row>
-    <row r="38" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>212</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>176</v>
+        <v>334</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>27</v>
       </c>
       <c r="G38" s="13">
-        <v>42076</v>
+        <v>42108</v>
       </c>
       <c r="H38" s="26" t="s">
         <v>24</v>
@@ -4085,27 +4112,27 @@
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>249</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>304</v>
+        <v>216</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>212</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>176</v>
+        <v>335</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F39" s="11" t="s">
         <v>27</v>
       </c>
       <c r="G39" s="13">
-        <v>42076</v>
+        <v>42108</v>
       </c>
       <c r="H39" s="26" t="s">
         <v>24</v>
@@ -4121,12 +4148,12 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>250</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>212</v>
@@ -4156,84 +4183,64 @@
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
-      <c r="T40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>325</v>
+        <v>303</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>76</v>
+        <v>233</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G41" s="13">
-        <v>42097</v>
+        <v>42076</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I41" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="J41" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M41" s="33">
-        <v>42097</v>
-      </c>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
       <c r="N41" s="10"/>
-      <c r="O41" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="O41" s="10"/>
       <c r="P41" s="10"/>
-      <c r="T41" t="s">
-        <v>34</v>
-      </c>
-      <c r="U41" s="31">
-        <f>COUNTIF(L2:L65,"*Minor*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>327</v>
+        <v>221</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>76</v>
+        <v>233</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G42" s="13">
-        <v>42097</v>
+        <v>42076</v>
       </c>
       <c r="H42" s="26" t="s">
         <v>24</v>
@@ -4241,61 +4248,111 @@
       <c r="I42" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="33"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
       <c r="N42" s="10"/>
-      <c r="O42" s="3"/>
+      <c r="O42" s="10"/>
       <c r="P42" s="10"/>
       <c r="T42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="13">
+        <v>42097</v>
+      </c>
+      <c r="H43" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M43" s="33">
+        <v>42097</v>
+      </c>
+      <c r="N43" s="10"/>
+      <c r="O43" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P43" s="10"/>
+      <c r="T43" t="s">
+        <v>34</v>
+      </c>
+      <c r="U43" s="31">
+        <f>COUNTIF(L2:L67,"*Minor*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="13">
+        <v>42097</v>
+      </c>
+      <c r="H44" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" s="3"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="10"/>
+      <c r="T44" t="s">
         <v>57</v>
       </c>
-      <c r="U42" s="31">
+      <c r="U44" s="31">
         <f>COUNTIF(L2:L21,"*Moderate*")</f>
         <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E43" s="10"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="T43" t="s">
-        <v>35</v>
-      </c>
-      <c r="U43" s="31">
-        <f>COUNTIF(L2:L21,"*Major*")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E44" s="10"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="T44" t="s">
-        <v>36</v>
-      </c>
-      <c r="U44" s="31">
-        <f>COUNTIF(L2:L21,"*Critical*")</f>
-        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
@@ -4312,11 +4369,11 @@
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
       <c r="T45" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="U45" s="31">
-        <f>COUNTIF(L2:L21,"*Cometic*")</f>
-        <v>0</v>
+        <f>COUNTIF(L2:L21,"*Major*")</f>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -4332,6 +4389,13 @@
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
       <c r="P46" s="10"/>
+      <c r="T46" t="s">
+        <v>36</v>
+      </c>
+      <c r="U46" s="31">
+        <f>COUNTIF(L2:L21,"*Critical*")</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E47" s="10"/>
@@ -4346,6 +4410,13 @@
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
+      <c r="T47" t="s">
+        <v>38</v>
+      </c>
+      <c r="U47" s="31">
+        <f>COUNTIF(L2:L21,"*Cometic*")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E48" s="10"/>
@@ -6101,7 +6172,7 @@
       <c r="E173" s="10"/>
       <c r="F173" s="11"/>
       <c r="G173" s="10"/>
-      <c r="H173" s="10"/>
+      <c r="H173" s="26"/>
       <c r="I173" s="10"/>
       <c r="J173" s="10"/>
       <c r="K173" s="10"/>
@@ -6115,7 +6186,7 @@
       <c r="E174" s="10"/>
       <c r="F174" s="11"/>
       <c r="G174" s="10"/>
-      <c r="H174" s="10"/>
+      <c r="H174" s="26"/>
       <c r="I174" s="10"/>
       <c r="J174" s="10"/>
       <c r="K174" s="10"/>
@@ -6127,7 +6198,7 @@
     </row>
     <row r="175" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E175" s="10"/>
-      <c r="F175" s="10"/>
+      <c r="F175" s="11"/>
       <c r="G175" s="10"/>
       <c r="H175" s="10"/>
       <c r="I175" s="10"/>
@@ -6141,7 +6212,7 @@
     </row>
     <row r="176" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E176" s="10"/>
-      <c r="F176" s="10"/>
+      <c r="F176" s="11"/>
       <c r="G176" s="10"/>
       <c r="H176" s="10"/>
       <c r="I176" s="10"/>
@@ -6153,10 +6224,38 @@
       <c r="O176" s="10"/>
       <c r="P176" s="10"/>
     </row>
+    <row r="177" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E177" s="10"/>
+      <c r="F177" s="10"/>
+      <c r="G177" s="10"/>
+      <c r="H177" s="10"/>
+      <c r="I177" s="10"/>
+      <c r="J177" s="10"/>
+      <c r="K177" s="10"/>
+      <c r="L177" s="10"/>
+      <c r="M177" s="10"/>
+      <c r="N177" s="10"/>
+      <c r="O177" s="10"/>
+      <c r="P177" s="10"/>
+    </row>
+    <row r="178" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E178" s="10"/>
+      <c r="F178" s="10"/>
+      <c r="G178" s="10"/>
+      <c r="H178" s="10"/>
+      <c r="I178" s="10"/>
+      <c r="J178" s="10"/>
+      <c r="K178" s="10"/>
+      <c r="L178" s="10"/>
+      <c r="M178" s="10"/>
+      <c r="N178" s="10"/>
+      <c r="O178" s="10"/>
+      <c r="P178" s="10"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H59:H174">
+  <conditionalFormatting sqref="H61:H176">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Passed ">
-      <formula>NOT(ISERROR(SEARCH("Passed ",H59)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Passed ",H61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6170,25 +6269,25 @@
           <x14:formula1>
             <xm:f>Settings!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H58</xm:sqref>
+          <xm:sqref>H2:H60</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F174</xm:sqref>
+          <xm:sqref>F2:F176</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$F$4:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L21 L26 L41:L42</xm:sqref>
+          <xm:sqref>L2:L21 L26 L43:L44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K26 K41:K42</xm:sqref>
+          <xm:sqref>K2:K26 K43:K44</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6201,10 +6300,10 @@
   <sheetPr>
     <tabColor rgb="FF99FF99"/>
   </sheetPr>
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6746,35 +6845,35 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>122</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>235</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>122</v>
@@ -6782,7 +6881,7 @@
     </row>
     <row r="25" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>236</v>
@@ -6791,7 +6890,7 @@
         <v>205</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>122</v>
@@ -6799,33 +6898,33 @@
     </row>
     <row r="26" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>237</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>238</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>122</v>
@@ -6833,16 +6932,16 @@
     </row>
     <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>239</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>122</v>
@@ -6850,16 +6949,16 @@
     </row>
     <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>240</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>122</v>
@@ -6867,16 +6966,16 @@
     </row>
     <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>241</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>122</v>
@@ -6884,7 +6983,7 @@
     </row>
     <row r="31" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>242</v>
@@ -6893,7 +6992,7 @@
         <v>213</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>122</v>
@@ -6901,7 +7000,7 @@
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>243</v>
@@ -6910,7 +7009,7 @@
         <v>214</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>122</v>
@@ -6918,7 +7017,7 @@
     </row>
     <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>244</v>
@@ -6927,7 +7026,7 @@
         <v>215</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>122</v>
@@ -6935,137 +7034,171 @@
     </row>
     <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>245</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>246</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>247</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>248</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>301</v>
+        <v>340</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>303</v>
+        <v>341</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>250</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="D40" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E42" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>122</v>
       </c>
     </row>
@@ -7161,21 +7294,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -7289,17 +7407,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7313,17 +7447,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>